<commit_message>
added landing probabilities to plots
</commit_message>
<xml_diff>
--- a/property_attributes.xlsx
+++ b/property_attributes.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,22 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodrigo.revilla\Desktop\monopoly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A97E0A0A-0EAD-4F19-B421-0612807A0CE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B2506B-08E3-423A-9263-227AF1576835}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="percentage per space" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$O$29</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="67">
   <si>
     <t>Mediterranean Avenue</t>
   </si>
@@ -97,48 +108,18 @@
     <t>St. Charles Place</t>
   </si>
   <si>
-    <t>rent with one house</t>
-  </si>
-  <si>
-    <t>rent with two houses</t>
-  </si>
-  <si>
-    <t>rent with three houses</t>
-  </si>
-  <si>
-    <t>rent with four houses</t>
-  </si>
-  <si>
-    <t>rent with hotel</t>
-  </si>
-  <si>
     <t>rent</t>
   </si>
   <si>
-    <t>monopoly rent</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
-    <t>group color</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>printed price</t>
-  </si>
-  <si>
-    <t>mortgage value</t>
-  </si>
-  <si>
-    <t>building costs</t>
-  </si>
-  <si>
     <t>brown</t>
   </si>
   <si>
@@ -191,12 +172,75 @@
   </si>
   <si>
     <t>dice x 10</t>
+  </si>
+  <si>
+    <t>monopoly_rent</t>
+  </si>
+  <si>
+    <t>rent_with_one_house</t>
+  </si>
+  <si>
+    <t>rent_with_two_houses</t>
+  </si>
+  <si>
+    <t>rent_with_three_houses</t>
+  </si>
+  <si>
+    <t>rent_with_four_houses</t>
+  </si>
+  <si>
+    <t>rent_with_hotel</t>
+  </si>
+  <si>
+    <t>printed_price</t>
+  </si>
+  <si>
+    <t>mortgage_value</t>
+  </si>
+  <si>
+    <t>building_costs</t>
+  </si>
+  <si>
+    <t>group_color</t>
+  </si>
+  <si>
+    <t>color_code</t>
+  </si>
+  <si>
+    <t>#955437</t>
+  </si>
+  <si>
+    <t>#aadff9</t>
+  </si>
+  <si>
+    <t>#d93a96</t>
+  </si>
+  <si>
+    <t>#f0932d</t>
+  </si>
+  <si>
+    <t>#ed1b24</t>
+  </si>
+  <si>
+    <t>#fef200</t>
+  </si>
+  <si>
+    <t>#22af5b</t>
+  </si>
+  <si>
+    <t>#0072ba</t>
+  </si>
+  <si>
+    <t>percentage</t>
+  </si>
+  <si>
+    <t>landing_probability</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
@@ -1037,1378 +1081,1843 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="8" width="19.140625" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" customWidth="1"/>
-    <col min="10" max="10" width="20.28515625" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="9" width="19.140625" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" customWidth="1"/>
+    <col min="16" max="16" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G1" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="H1" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="I1" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="J1" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="K1" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="L1" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="M1" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="N1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="O1" t="s">
+        <v>54</v>
+      </c>
+      <c r="P1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="2">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="2">
         <v>1</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>2</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>4</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <v>10</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I2" s="2">
         <v>30</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <v>90</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <v>160</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <v>250</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>60</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>30</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P2">
+        <f>VLOOKUP(E2,'percentage per space'!$A$2:$B$42,2,0)</f>
+        <v>1.9532251197312001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3</v>
+      </c>
+      <c r="F3" s="2">
+        <v>4</v>
+      </c>
+      <c r="G3" s="2">
+        <v>8</v>
+      </c>
+      <c r="H3" s="2">
+        <v>20</v>
+      </c>
+      <c r="I3" s="2">
+        <v>60</v>
+      </c>
+      <c r="J3" s="2">
+        <v>180</v>
+      </c>
+      <c r="K3" s="2">
+        <v>320</v>
+      </c>
+      <c r="L3" s="2">
+        <v>450</v>
+      </c>
+      <c r="M3">
+        <v>60</v>
+      </c>
+      <c r="N3">
+        <v>30</v>
+      </c>
+      <c r="O3">
+        <v>50</v>
+      </c>
+      <c r="P3">
+        <f>VLOOKUP(E3,'percentage per space'!$A$2:$B$42,2,0)</f>
+        <v>2.01300155931552E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="2">
-        <v>3</v>
-      </c>
-      <c r="E3" s="2">
-        <v>4</v>
-      </c>
-      <c r="F3" s="2">
-        <v>8</v>
-      </c>
-      <c r="G3" s="2">
-        <v>20</v>
-      </c>
-      <c r="H3" s="2">
-        <v>60</v>
-      </c>
-      <c r="I3" s="2">
-        <v>180</v>
-      </c>
-      <c r="J3" s="2">
-        <v>320</v>
-      </c>
-      <c r="K3" s="2">
-        <v>450</v>
-      </c>
-      <c r="L3">
-        <v>60</v>
-      </c>
-      <c r="M3">
-        <v>30</v>
-      </c>
-      <c r="N3">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>48</v>
-      </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="2">
+        <v>42</v>
+      </c>
+      <c r="E4" s="2">
         <v>5</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>25</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>200</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="L4">
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4">
         <v>200</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>100</v>
       </c>
-      <c r="N4" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="O4" s="2"/>
+      <c r="P4">
+        <f>VLOOKUP(E4,'percentage per space'!$A$2:$B$42,2,0)</f>
+        <v>2.6434136829427302E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="2">
-        <v>6</v>
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>58</v>
       </c>
       <c r="E5" s="2">
         <v>6</v>
       </c>
       <c r="F5" s="2">
+        <v>6</v>
+      </c>
+      <c r="G5" s="2">
         <v>12</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>30</v>
       </c>
-      <c r="H5" s="2">
+      <c r="I5" s="2">
         <v>90</v>
       </c>
-      <c r="I5" s="2">
+      <c r="J5" s="2">
         <v>270</v>
       </c>
-      <c r="J5" s="2">
+      <c r="K5" s="2">
         <v>400</v>
       </c>
-      <c r="K5" s="2">
+      <c r="L5" s="2">
         <v>550</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>100</v>
-      </c>
-      <c r="M5">
-        <v>50</v>
       </c>
       <c r="N5">
         <v>50</v>
       </c>
-      <c r="T5" s="1"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="O5">
+        <v>50</v>
+      </c>
+      <c r="P5">
+        <f>VLOOKUP(E5,'percentage per space'!$A$2:$B$42,2,0)</f>
+        <v>2.1403719830489699E-2</v>
+      </c>
+      <c r="U5" s="1"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="2">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="2">
         <v>8</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>6</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <v>12</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>30</v>
       </c>
-      <c r="H6" s="2">
+      <c r="I6" s="2">
         <v>90</v>
       </c>
-      <c r="I6" s="2">
+      <c r="J6" s="2">
         <v>270</v>
       </c>
-      <c r="J6" s="2">
+      <c r="K6" s="2">
         <v>400</v>
       </c>
-      <c r="K6" s="2">
+      <c r="L6" s="2">
         <v>550</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>100</v>
-      </c>
-      <c r="M6">
-        <v>50</v>
       </c>
       <c r="N6">
         <v>50</v>
       </c>
-      <c r="T6" s="1"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="O6">
+        <v>50</v>
+      </c>
+      <c r="P6">
+        <f>VLOOKUP(E6,'percentage per space'!$A$2:$B$42,2,0)</f>
+        <v>2.1861397433266601E-2</v>
+      </c>
+      <c r="U6" s="1"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="2">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="2">
         <v>9</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>8</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7" s="2">
         <v>16</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="2">
         <v>40</v>
       </c>
-      <c r="H7" s="2">
+      <c r="I7" s="2">
         <v>100</v>
       </c>
-      <c r="I7" s="2">
+      <c r="J7" s="2">
         <v>300</v>
       </c>
-      <c r="J7" s="2">
+      <c r="K7" s="2">
         <v>450</v>
       </c>
-      <c r="K7" s="2">
+      <c r="L7" s="2">
         <v>600</v>
       </c>
-      <c r="L7" s="2">
+      <c r="M7" s="2">
         <v>120</v>
       </c>
-      <c r="M7" s="2">
+      <c r="N7" s="2">
         <v>60</v>
       </c>
-      <c r="N7" s="2">
+      <c r="O7" s="2">
         <v>50</v>
       </c>
-      <c r="T7" s="1"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P7">
+        <f>VLOOKUP(E7,'percentage per space'!$A$2:$B$42,2,0)</f>
+        <v>2.15592379215752E-2</v>
+      </c>
+      <c r="U7" s="1"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="2">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="2">
         <v>11</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>10</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <v>20</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>50</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I8" s="2">
         <v>150</v>
       </c>
-      <c r="I8" s="2">
+      <c r="J8" s="2">
         <v>450</v>
       </c>
-      <c r="J8" s="2">
+      <c r="K8" s="2">
         <v>625</v>
       </c>
-      <c r="K8" s="2">
+      <c r="L8" s="2">
         <v>750</v>
       </c>
-      <c r="L8" s="2">
+      <c r="M8" s="2">
         <v>140</v>
       </c>
-      <c r="M8" s="2">
+      <c r="N8" s="2">
         <v>70</v>
       </c>
-      <c r="N8" s="2">
+      <c r="O8" s="2">
         <v>100</v>
       </c>
-      <c r="T8" s="1"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P8">
+        <f>VLOOKUP(E8,'percentage per space'!$A$2:$B$42,2,0)</f>
+        <v>2.5246191418481799E-2</v>
+      </c>
+      <c r="U8" s="1"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="2">
+        <v>42</v>
+      </c>
+      <c r="E9" s="2">
         <v>12</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="F9" s="2" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="L9" s="2">
+        <v>45</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2">
         <v>150</v>
       </c>
-      <c r="M9" s="2">
+      <c r="N9" s="2">
         <v>75</v>
       </c>
-      <c r="N9" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="T9" s="1"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="O9" s="2"/>
+      <c r="P9">
+        <f>VLOOKUP(E9,'percentage per space'!$A$2:$B$42,2,0)</f>
+        <v>2.42505248796809E-2</v>
+      </c>
+      <c r="U9" s="1"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="2">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="2">
         <v>13</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F10" s="2">
         <v>10</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G10" s="2">
         <v>20</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" s="2">
         <v>50</v>
       </c>
-      <c r="H10" s="2">
+      <c r="I10" s="2">
         <v>150</v>
       </c>
-      <c r="I10" s="2">
+      <c r="J10" s="2">
         <v>450</v>
       </c>
-      <c r="J10" s="2">
+      <c r="K10" s="2">
         <v>625</v>
       </c>
-      <c r="K10" s="2">
+      <c r="L10" s="2">
         <v>750</v>
       </c>
-      <c r="L10" s="2">
+      <c r="M10" s="2">
         <v>140</v>
       </c>
-      <c r="M10" s="2">
+      <c r="N10" s="2">
         <v>70</v>
       </c>
-      <c r="N10" s="2">
+      <c r="O10" s="2">
         <v>100</v>
       </c>
-      <c r="T10" s="1"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P10">
+        <f>VLOOKUP(E10,'percentage per space'!$A$2:$B$42,2,0)</f>
+        <v>2.2050443081064498E-2</v>
+      </c>
+      <c r="U10" s="1"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="2">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="2">
         <v>14</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F11" s="2">
         <v>12</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G11" s="2">
         <v>24</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H11" s="2">
         <v>60</v>
       </c>
-      <c r="H11" s="2">
+      <c r="I11" s="2">
         <v>180</v>
       </c>
-      <c r="I11" s="2">
+      <c r="J11" s="2">
         <v>500</v>
       </c>
-      <c r="J11" s="2">
+      <c r="K11" s="2">
         <v>700</v>
       </c>
-      <c r="K11" s="2">
+      <c r="L11" s="2">
         <v>900</v>
       </c>
-      <c r="L11" s="2">
+      <c r="M11" s="2">
         <v>160</v>
       </c>
-      <c r="M11" s="2">
+      <c r="N11" s="2">
         <v>80</v>
       </c>
-      <c r="N11" s="2">
+      <c r="O11" s="2">
         <v>100</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P11">
+        <f>VLOOKUP(E11,'percentage per space'!$A$2:$B$42,2,0)</f>
+        <v>2.29711086126669E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="2">
+        <v>42</v>
+      </c>
+      <c r="E12" s="2">
         <v>15</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F12" s="2">
         <v>25</v>
       </c>
-      <c r="F12" s="2">
+      <c r="G12" s="2">
         <v>200</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="L12">
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12">
         <v>200</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>100</v>
       </c>
-      <c r="N12" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="T12" s="1"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="O12" s="2"/>
+      <c r="P12">
+        <f>VLOOKUP(E12,'percentage per space'!$A$2:$B$42,2,0)</f>
+        <v>2.5878796256075101E-2</v>
+      </c>
+      <c r="U12" s="1"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="2">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="2">
         <v>16</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F13" s="2">
         <v>14</v>
       </c>
-      <c r="F13" s="2">
+      <c r="G13" s="2">
         <v>28</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H13" s="2">
         <v>70</v>
       </c>
-      <c r="H13" s="2">
+      <c r="I13" s="2">
         <v>200</v>
       </c>
-      <c r="I13" s="2">
+      <c r="J13" s="2">
         <v>550</v>
       </c>
-      <c r="J13" s="2">
+      <c r="K13" s="2">
         <v>750</v>
       </c>
-      <c r="K13" s="2">
+      <c r="L13" s="2">
         <v>950</v>
       </c>
-      <c r="L13" s="2">
+      <c r="M13" s="2">
         <v>180</v>
       </c>
-      <c r="M13" s="2">
+      <c r="N13" s="2">
         <v>90</v>
       </c>
-      <c r="N13" s="2">
+      <c r="O13" s="2">
         <v>100</v>
       </c>
-      <c r="S13" s="1"/>
+      <c r="P13">
+        <f>VLOOKUP(E13,'percentage per space'!$A$2:$B$42,2,0)</f>
+        <v>2.5948457544276399E-2</v>
+      </c>
       <c r="T13" s="1"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U13" s="1"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="2">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="2">
         <v>18</v>
       </c>
-      <c r="E14" s="2">
+      <c r="F14" s="2">
         <v>14</v>
       </c>
-      <c r="F14" s="2">
+      <c r="G14" s="2">
         <v>28</v>
       </c>
-      <c r="G14" s="2">
+      <c r="H14" s="2">
         <v>70</v>
       </c>
-      <c r="H14" s="2">
+      <c r="I14" s="2">
         <v>200</v>
       </c>
-      <c r="I14" s="2">
+      <c r="J14" s="2">
         <v>550</v>
       </c>
-      <c r="J14" s="2">
+      <c r="K14" s="2">
         <v>750</v>
       </c>
-      <c r="K14" s="2">
+      <c r="L14" s="2">
         <v>950</v>
       </c>
-      <c r="L14" s="2">
+      <c r="M14" s="2">
         <v>180</v>
       </c>
-      <c r="M14" s="2">
+      <c r="N14" s="2">
         <v>90</v>
       </c>
-      <c r="N14" s="2">
+      <c r="O14" s="2">
         <v>100</v>
       </c>
-      <c r="S14" s="1"/>
+      <c r="P14">
+        <f>VLOOKUP(E14,'percentage per space'!$A$2:$B$42,2,0)</f>
+        <v>2.7142212961396801E-2</v>
+      </c>
       <c r="T14" s="1"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U14" s="1"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="2">
+        <v>31</v>
+      </c>
+      <c r="D15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="2">
         <v>19</v>
       </c>
-      <c r="E15" s="2">
+      <c r="F15" s="2">
         <v>16</v>
       </c>
-      <c r="F15" s="2">
+      <c r="G15" s="2">
         <v>32</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H15" s="2">
         <v>80</v>
       </c>
-      <c r="H15" s="2">
+      <c r="I15" s="2">
         <v>220</v>
       </c>
-      <c r="I15" s="2">
+      <c r="J15" s="2">
         <v>600</v>
       </c>
-      <c r="J15" s="2">
+      <c r="K15" s="2">
         <v>800</v>
       </c>
-      <c r="K15" s="2">
+      <c r="L15" s="2">
         <v>1000</v>
       </c>
-      <c r="L15" s="2">
+      <c r="M15" s="2">
         <v>200</v>
-      </c>
-      <c r="M15" s="2">
-        <v>100</v>
       </c>
       <c r="N15" s="2">
         <v>100</v>
       </c>
-      <c r="Q15" s="1"/>
-      <c r="S15" s="1"/>
+      <c r="O15" s="2">
+        <v>100</v>
+      </c>
+      <c r="P15">
+        <f>VLOOKUP(E15,'percentage per space'!$A$2:$B$42,2,0)</f>
+        <v>2.8449317385999599E-2</v>
+      </c>
+      <c r="R15" s="1"/>
       <c r="T15" s="1"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U15" s="1"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="2">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="2">
         <v>21</v>
       </c>
-      <c r="E16" s="2">
+      <c r="F16" s="2">
         <v>18</v>
       </c>
-      <c r="F16" s="2">
+      <c r="G16" s="2">
         <v>36</v>
       </c>
-      <c r="G16" s="2">
+      <c r="H16" s="2">
         <v>90</v>
       </c>
-      <c r="H16" s="2">
+      <c r="I16" s="2">
         <v>250</v>
       </c>
-      <c r="I16" s="2">
+      <c r="J16" s="2">
         <v>700</v>
       </c>
-      <c r="J16" s="2">
+      <c r="K16" s="2">
         <v>875</v>
       </c>
-      <c r="K16" s="2">
+      <c r="L16" s="2">
         <v>1050</v>
       </c>
-      <c r="L16" s="2">
+      <c r="M16" s="2">
         <v>220</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>110</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <v>150</v>
       </c>
-      <c r="Q16" s="1"/>
-      <c r="S16" s="1"/>
+      <c r="P16">
+        <f>VLOOKUP(E16,'percentage per space'!$A$2:$B$42,2,0)</f>
+        <v>2.60691058006631E-2</v>
+      </c>
+      <c r="R16" s="1"/>
       <c r="T16" s="1"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U16" s="1"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="2">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="2">
         <v>23</v>
       </c>
-      <c r="E17" s="2">
+      <c r="F17" s="2">
         <v>18</v>
       </c>
-      <c r="F17" s="2">
+      <c r="G17" s="2">
         <v>36</v>
       </c>
-      <c r="G17" s="2">
+      <c r="H17" s="2">
         <v>90</v>
       </c>
-      <c r="H17" s="2">
+      <c r="I17" s="2">
         <v>250</v>
       </c>
-      <c r="I17" s="2">
+      <c r="J17" s="2">
         <v>700</v>
       </c>
-      <c r="J17" s="2">
+      <c r="K17" s="2">
         <v>875</v>
       </c>
-      <c r="K17" s="2">
+      <c r="L17" s="2">
         <v>1050</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>220</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>110</v>
       </c>
-      <c r="N17">
+      <c r="O17">
         <v>150</v>
       </c>
-      <c r="Q17" s="1"/>
-      <c r="S17" s="1"/>
+      <c r="P17">
+        <f>VLOOKUP(E17,'percentage per space'!$A$2:$B$42,2,0)</f>
+        <v>2.50854805731421E-2</v>
+      </c>
+      <c r="R17" s="1"/>
       <c r="T17" s="1"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U17" s="1"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="2">
+        <v>24</v>
+      </c>
+      <c r="F18" s="2">
+        <v>20</v>
+      </c>
+      <c r="G18" s="2">
+        <v>40</v>
+      </c>
+      <c r="H18" s="2">
+        <v>100</v>
+      </c>
+      <c r="I18" s="2">
+        <v>300</v>
+      </c>
+      <c r="J18" s="2">
+        <v>750</v>
+      </c>
+      <c r="K18" s="2">
+        <v>925</v>
+      </c>
+      <c r="L18" s="2">
+        <v>1100</v>
+      </c>
+      <c r="M18" s="2">
+        <v>240</v>
+      </c>
+      <c r="N18" s="2">
+        <v>120</v>
+      </c>
+      <c r="O18" s="2">
+        <v>150</v>
+      </c>
+      <c r="P18">
+        <f>VLOOKUP(E18,'percentage per space'!$A$2:$B$42,2,0)</f>
+        <v>2.9317487111387999E-2</v>
+      </c>
+      <c r="R18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" t="s">
         <v>42</v>
-      </c>
-      <c r="D18" s="2">
-        <v>24</v>
-      </c>
-      <c r="E18" s="2">
-        <v>20</v>
-      </c>
-      <c r="F18" s="2">
-        <v>40</v>
-      </c>
-      <c r="G18" s="2">
-        <v>100</v>
-      </c>
-      <c r="H18" s="2">
-        <v>300</v>
-      </c>
-      <c r="I18" s="2">
-        <v>750</v>
-      </c>
-      <c r="J18" s="2">
-        <v>925</v>
-      </c>
-      <c r="K18" s="2">
-        <v>1100</v>
-      </c>
-      <c r="L18" s="2">
-        <v>240</v>
-      </c>
-      <c r="M18" s="2">
-        <v>120</v>
-      </c>
-      <c r="N18" s="2">
-        <v>150</v>
-      </c>
-      <c r="Q18" s="1"/>
-      <c r="S18" s="1"/>
-      <c r="T18" s="1"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19" s="2">
-        <v>25</v>
       </c>
       <c r="E19" s="2">
         <v>25</v>
       </c>
       <c r="F19" s="2">
+        <v>25</v>
+      </c>
+      <c r="G19" s="2">
         <v>200</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="L19">
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19">
         <v>200</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <v>100</v>
       </c>
-      <c r="N19" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q19" s="1"/>
-      <c r="S19" s="1"/>
+      <c r="O19" s="2"/>
+      <c r="P19">
+        <f>VLOOKUP(E19,'percentage per space'!$A$2:$B$42,2,0)</f>
+        <v>2.65853733476656E-2</v>
+      </c>
+      <c r="R19" s="1"/>
       <c r="T19" s="1"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U19" s="1"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="2">
+        <v>33</v>
+      </c>
+      <c r="D20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="2">
         <v>26</v>
       </c>
-      <c r="E20" s="2">
+      <c r="F20" s="2">
         <v>22</v>
       </c>
-      <c r="F20" s="2">
+      <c r="G20" s="2">
         <v>44</v>
       </c>
-      <c r="G20" s="2">
+      <c r="H20" s="2">
         <v>110</v>
       </c>
-      <c r="H20" s="2">
+      <c r="I20" s="2">
         <v>330</v>
       </c>
-      <c r="I20" s="2">
+      <c r="J20" s="2">
         <v>800</v>
       </c>
-      <c r="J20" s="2">
+      <c r="K20" s="2">
         <v>975</v>
       </c>
-      <c r="K20" s="2">
+      <c r="L20" s="2">
         <v>1150</v>
       </c>
-      <c r="L20" s="2">
+      <c r="M20" s="2">
         <v>260</v>
       </c>
-      <c r="M20" s="2">
+      <c r="N20" s="2">
         <v>130</v>
       </c>
-      <c r="N20" s="2">
+      <c r="O20" s="2">
         <v>150</v>
       </c>
-      <c r="Q20" s="1"/>
-      <c r="S20" s="1"/>
+      <c r="P20">
+        <f>VLOOKUP(E20,'percentage per space'!$A$2:$B$42,2,0)</f>
+        <v>2.4943140320682601E-2</v>
+      </c>
+      <c r="R20" s="1"/>
       <c r="T20" s="1"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U20" s="1"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="2">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="2">
         <v>27</v>
       </c>
-      <c r="E21" s="2">
+      <c r="F21" s="2">
         <v>22</v>
       </c>
-      <c r="F21" s="2">
+      <c r="G21" s="2">
         <v>44</v>
       </c>
-      <c r="G21" s="2">
+      <c r="H21" s="2">
         <v>110</v>
       </c>
-      <c r="H21" s="2">
+      <c r="I21" s="2">
         <v>330</v>
       </c>
-      <c r="I21" s="2">
+      <c r="J21" s="2">
         <v>800</v>
       </c>
-      <c r="J21" s="2">
+      <c r="K21" s="2">
         <v>975</v>
       </c>
-      <c r="K21" s="2">
+      <c r="L21" s="2">
         <v>1150</v>
       </c>
-      <c r="L21" s="2">
+      <c r="M21" s="2">
         <v>260</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <v>130</v>
       </c>
-      <c r="N21">
+      <c r="O21">
         <v>150</v>
       </c>
-      <c r="Q21" s="1"/>
-      <c r="T21" s="1"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P21">
+        <f>VLOOKUP(E21,'percentage per space'!$A$2:$B$42,2,0)</f>
+        <v>2.47093586051031E-2</v>
+      </c>
+      <c r="R21" s="1"/>
+      <c r="U21" s="1"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C22" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="2">
+        <v>42</v>
+      </c>
+      <c r="E22" s="2">
         <v>28</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="F22" s="2" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="L22" s="2">
+        <v>45</v>
+      </c>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2">
         <v>150</v>
       </c>
-      <c r="M22" s="2">
+      <c r="N22" s="2">
         <v>75</v>
       </c>
-      <c r="N22" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q22" s="1"/>
-      <c r="T22" s="1"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="O22" s="2"/>
+      <c r="P22">
+        <f>VLOOKUP(E22,'percentage per space'!$A$2:$B$42,2,0)</f>
+        <v>2.5845944737180802E-2</v>
+      </c>
+      <c r="R22" s="1"/>
+      <c r="U22" s="1"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" s="2">
+        <v>33</v>
+      </c>
+      <c r="D23" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" s="2">
         <v>29</v>
       </c>
-      <c r="E23" s="2">
+      <c r="F23" s="2">
         <v>24</v>
       </c>
-      <c r="F23" s="2">
+      <c r="G23" s="2">
         <v>48</v>
       </c>
-      <c r="G23" s="2">
+      <c r="H23" s="2">
         <v>120</v>
       </c>
-      <c r="H23" s="2">
+      <c r="I23" s="2">
         <v>360</v>
       </c>
-      <c r="I23" s="2">
+      <c r="J23" s="2">
         <v>850</v>
       </c>
-      <c r="J23" s="2">
+      <c r="K23" s="2">
         <v>1025</v>
       </c>
-      <c r="K23" s="2">
+      <c r="L23" s="2">
         <v>1200</v>
       </c>
-      <c r="L23" s="2">
+      <c r="M23" s="2">
         <v>280</v>
       </c>
-      <c r="M23" s="2">
+      <c r="N23" s="2">
         <v>140</v>
       </c>
-      <c r="N23" s="2">
+      <c r="O23" s="2">
         <v>150</v>
       </c>
-      <c r="T23" s="1"/>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P23">
+        <f>VLOOKUP(E23,'percentage per space'!$A$2:$B$42,2,0)</f>
+        <v>2.3810394867223E-2</v>
+      </c>
+      <c r="U23" s="1"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C24" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="2">
+        <v>34</v>
+      </c>
+      <c r="D24" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="2">
         <v>31</v>
       </c>
-      <c r="E24" s="2">
+      <c r="F24" s="2">
         <v>26</v>
       </c>
-      <c r="F24" s="2">
+      <c r="G24" s="2">
         <v>52</v>
       </c>
-      <c r="G24" s="2">
+      <c r="H24" s="2">
         <v>130</v>
       </c>
-      <c r="H24" s="2">
+      <c r="I24" s="2">
         <v>390</v>
       </c>
-      <c r="I24" s="2">
+      <c r="J24" s="2">
         <v>900</v>
       </c>
-      <c r="J24" s="2">
+      <c r="K24" s="2">
         <v>1100</v>
       </c>
-      <c r="K24" s="2">
+      <c r="L24" s="2">
         <v>1275</v>
       </c>
-      <c r="L24" s="2">
+      <c r="M24" s="2">
         <v>300</v>
       </c>
-      <c r="M24" s="2">
+      <c r="N24" s="2">
         <v>150</v>
       </c>
-      <c r="N24" s="2">
+      <c r="O24" s="2">
         <v>200</v>
       </c>
-      <c r="T24" s="1"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P24">
+        <f>VLOOKUP(E24,'percentage per space'!$A$2:$B$42,2,0)</f>
+        <v>2.4498542580036201E-2</v>
+      </c>
+      <c r="U24" s="1"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C25" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" s="2">
+        <v>34</v>
+      </c>
+      <c r="D25" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="2">
         <v>32</v>
       </c>
-      <c r="E25" s="2">
+      <c r="F25" s="2">
         <v>26</v>
       </c>
-      <c r="F25" s="2">
+      <c r="G25" s="2">
         <v>52</v>
       </c>
-      <c r="G25" s="2">
+      <c r="H25" s="2">
         <v>130</v>
       </c>
-      <c r="H25" s="2">
+      <c r="I25" s="2">
         <v>390</v>
       </c>
-      <c r="I25" s="2">
+      <c r="J25" s="2">
         <v>900</v>
       </c>
-      <c r="J25" s="2">
+      <c r="K25" s="2">
         <v>1100</v>
       </c>
-      <c r="K25" s="2">
+      <c r="L25" s="2">
         <v>1275</v>
       </c>
-      <c r="L25" s="2">
+      <c r="M25" s="2">
         <v>300</v>
       </c>
-      <c r="M25" s="2">
+      <c r="N25" s="2">
         <v>150</v>
       </c>
-      <c r="N25" s="2">
+      <c r="O25" s="2">
         <v>200</v>
       </c>
-      <c r="T25" s="1"/>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P25">
+        <f>VLOOKUP(E25,'percentage per space'!$A$2:$B$42,2,0)</f>
+        <v>2.3935941948377799E-2</v>
+      </c>
+      <c r="U25" s="1"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>18</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C26" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" s="2">
         <v>34</v>
       </c>
+      <c r="D26" t="s">
+        <v>63</v>
+      </c>
       <c r="E26" s="2">
+        <v>34</v>
+      </c>
+      <c r="F26" s="2">
         <v>28</v>
       </c>
-      <c r="F26" s="2">
+      <c r="G26" s="2">
         <v>56</v>
       </c>
-      <c r="G26" s="2">
+      <c r="H26" s="2">
         <v>150</v>
       </c>
-      <c r="H26" s="2">
+      <c r="I26" s="2">
         <v>450</v>
       </c>
-      <c r="I26" s="2">
+      <c r="J26" s="2">
         <v>1000</v>
       </c>
-      <c r="J26" s="2">
+      <c r="K26" s="2">
         <v>1200</v>
       </c>
-      <c r="K26" s="2">
+      <c r="L26" s="2">
         <v>1400</v>
       </c>
-      <c r="L26" s="2">
+      <c r="M26" s="2">
         <v>320</v>
       </c>
-      <c r="M26" s="2">
+      <c r="N26" s="2">
         <v>160</v>
       </c>
-      <c r="N26" s="2">
+      <c r="O26" s="2">
         <v>200</v>
       </c>
-      <c r="T26" s="1"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P26">
+        <f>VLOOKUP(E26,'percentage per space'!$A$2:$B$42,2,0)</f>
+        <v>2.2831795833913999E-2</v>
+      </c>
+      <c r="U26" s="1"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C27" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" s="2">
+        <v>42</v>
+      </c>
+      <c r="E27" s="2">
         <v>35</v>
       </c>
-      <c r="E27" s="2">
+      <c r="F27" s="2">
         <v>25</v>
       </c>
-      <c r="F27" s="2">
+      <c r="G27" s="2">
         <v>200</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="L27">
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27">
         <v>200</v>
       </c>
-      <c r="M27">
+      <c r="N27">
         <v>100</v>
       </c>
-      <c r="N27" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="T27" s="1"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="O27" s="2"/>
+      <c r="P27">
+        <f>VLOOKUP(E27,'percentage per space'!$A$2:$B$42,2,0)</f>
+        <v>2.22283194083913E-2</v>
+      </c>
+      <c r="U27" s="1"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>19</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C28" t="s">
-        <v>45</v>
-      </c>
-      <c r="D28" s="2">
+        <v>35</v>
+      </c>
+      <c r="D28" t="s">
+        <v>64</v>
+      </c>
+      <c r="E28" s="2">
         <v>37</v>
       </c>
-      <c r="E28" s="2">
+      <c r="F28" s="2">
         <v>35</v>
       </c>
-      <c r="F28" s="2">
+      <c r="G28" s="2">
         <v>70</v>
       </c>
-      <c r="G28" s="2">
+      <c r="H28" s="2">
         <v>175</v>
       </c>
-      <c r="H28" s="2">
+      <c r="I28" s="2">
         <v>500</v>
       </c>
-      <c r="I28" s="2">
+      <c r="J28" s="2">
         <v>1100</v>
       </c>
-      <c r="J28" s="2">
+      <c r="K28" s="2">
         <v>1300</v>
       </c>
-      <c r="K28" s="2">
+      <c r="L28" s="2">
         <v>1500</v>
       </c>
-      <c r="L28" s="2">
+      <c r="M28" s="2">
         <v>350</v>
       </c>
-      <c r="M28" s="2">
+      <c r="N28" s="2">
         <v>175</v>
       </c>
-      <c r="N28" s="2">
+      <c r="O28" s="2">
         <v>200</v>
       </c>
-      <c r="T28" s="1"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P28">
+        <f>VLOOKUP(E28,'percentage per space'!$A$2:$B$42,2,0)</f>
+        <v>1.9971558207208799E-2</v>
+      </c>
+      <c r="U28" s="1"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D29" s="2">
+        <v>35</v>
+      </c>
+      <c r="D29" t="s">
+        <v>64</v>
+      </c>
+      <c r="E29" s="2">
         <v>39</v>
       </c>
-      <c r="E29" s="2">
+      <c r="F29" s="2">
         <v>50</v>
       </c>
-      <c r="F29" s="2">
+      <c r="G29" s="2">
         <v>100</v>
       </c>
-      <c r="G29" s="2">
+      <c r="H29" s="2">
         <v>200</v>
       </c>
-      <c r="H29" s="2">
+      <c r="I29" s="2">
         <v>600</v>
       </c>
-      <c r="I29" s="2">
+      <c r="J29" s="2">
         <v>1400</v>
       </c>
-      <c r="J29" s="2">
+      <c r="K29" s="2">
         <v>1700</v>
       </c>
-      <c r="K29" s="2">
+      <c r="L29" s="2">
         <v>2000</v>
       </c>
-      <c r="L29" s="2">
+      <c r="M29" s="2">
         <v>400</v>
-      </c>
-      <c r="M29" s="2">
-        <v>200</v>
       </c>
       <c r="N29" s="2">
         <v>200</v>
       </c>
-      <c r="T29" s="1"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="M30" s="1"/>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="M31" s="1"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="M32" s="1"/>
-    </row>
-    <row r="33" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M33" s="1"/>
-    </row>
-    <row r="34" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M34" s="1"/>
-    </row>
-    <row r="35" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M35" s="1"/>
-    </row>
-    <row r="36" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M36" s="1"/>
-    </row>
-    <row r="37" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M37" s="1"/>
-    </row>
-    <row r="38" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M38" s="1"/>
+      <c r="O29" s="2">
+        <v>200</v>
+      </c>
+      <c r="P29">
+        <f>VLOOKUP(E29,'percentage per space'!$A$2:$B$42,2,0)</f>
+        <v>2.4088706899943701E-2</v>
+      </c>
+      <c r="U29" s="1"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="N30" s="1"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="N31" s="1"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="N32" s="1"/>
+    </row>
+    <row r="33" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N33" s="1"/>
+    </row>
+    <row r="34" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N34" s="1"/>
+    </row>
+    <row r="35" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N35" s="1"/>
+    </row>
+    <row r="36" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N36" s="1"/>
+    </row>
+    <row r="37" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N37" s="1"/>
+    </row>
+    <row r="38" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N38" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N29">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N29">
-      <sortCondition ref="D1:D29"/>
+  <autoFilter ref="A1:O29" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O29">
+      <sortCondition ref="E1:E29"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5723DB66-45DD-4475-AF61-AFF389B10402}">
+  <dimension ref="A1:B42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>3.2994731137604302E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1.9532251197312001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1.9898320776926999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>2.01300155931552E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2.1773022634451598E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2.6434136829427302E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>2.1403719830489699E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>2.1904252352337301E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>2.1861397433266601E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>2.15592379215752E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>2.1271823872435501E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>10.5</v>
+      </c>
+      <c r="B13">
+        <v>3.5565751947655197E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>2.5246191418481799E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>2.42505248796809E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>2.2050443081064498E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>2.29711086126669E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>2.5878796256075101E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>2.5948457544276399E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>2.7473647849901899E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>2.7142212961396801E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>2.8449317385999599E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>2.6544546542048901E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24">
+        <v>2.60691058006631E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25">
+        <v>2.5682490549971099E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26">
+        <v>2.50854805731421E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="B27">
+        <v>2.9317487111387999E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>25</v>
+      </c>
+      <c r="B28">
+        <v>2.65853733476656E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>26</v>
+      </c>
+      <c r="B29">
+        <v>2.4943140320682601E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>27</v>
+      </c>
+      <c r="B30">
+        <v>2.47093586051031E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>28</v>
+      </c>
+      <c r="B31">
+        <v>2.5845944737180802E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>29</v>
+      </c>
+      <c r="B32">
+        <v>2.3810394867223E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>30</v>
+      </c>
+      <c r="B33">
+        <v>2.43046275004189E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>31</v>
+      </c>
+      <c r="B34">
+        <v>2.4498542580036201E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>32</v>
+      </c>
+      <c r="B35">
+        <v>2.3935941948377799E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>33</v>
+      </c>
+      <c r="B36">
+        <v>2.4712748591842599E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>34</v>
+      </c>
+      <c r="B37">
+        <v>2.2831795833913999E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>35</v>
+      </c>
+      <c r="B38">
+        <v>2.22283194083913E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>36</v>
+      </c>
+      <c r="B39">
+        <v>2.1174748760832501E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>37</v>
+      </c>
+      <c r="B40">
+        <v>1.9971558207208799E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>38</v>
+      </c>
+      <c r="B41">
+        <v>1.99203262977849E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>39</v>
+      </c>
+      <c r="B42">
+        <v>2.4088706899943701E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>